<commit_message>
Add Files Upload and Update Data
</commit_message>
<xml_diff>
--- a/data/Employee.xlsx
+++ b/data/Employee.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Azwan Azlan\Desktop\playwright-project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C92402B-A5AB-4733-8B99-3A633142E51E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B40586D-A735-4687-8363-086C53830D32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t xml:space="preserve">First Name </t>
   </si>
@@ -49,6 +49,18 @@
   </si>
   <si>
     <t>Parker</t>
+  </si>
+  <si>
+    <t>Path</t>
+  </si>
+  <si>
+    <t>./data/Tony Stark.jpg</t>
+  </si>
+  <si>
+    <t>./data/Tom Hank.jpg</t>
+  </si>
+  <si>
+    <t>./data/Peter Parker.jpg</t>
   </si>
 </sst>
 </file>
@@ -84,8 +96,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -366,50 +379,62 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15.42578125" customWidth="1"/>
-    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" customWidth="1"/>
     <col min="4" max="4" width="16.42578125" customWidth="1"/>
     <col min="5" max="5" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
+      <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>